<commit_message>
Convert xslx to csv
</commit_message>
<xml_diff>
--- a/data/batch1/Dataset1_Prior_Therapy_Trials_First.xlsx
+++ b/data/batch1/Dataset1_Prior_Therapy_Trials_First.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Documents/GitHub/tophealth/data/batch1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muchniki/dev/tophealthai/tophealth.github.io/data/batch1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Logic" sheetId="1" r:id="rId1"/>
+    <sheet name="Codes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$308</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Logic!$A$1:$F$308</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -6220,7 +6220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F312"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -11491,7 +11491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>